<commit_message>
add alison suggests, play w ML in wea
</commit_message>
<xml_diff>
--- a/_data/lit/lit_summary-penalty-over-years.xlsx
+++ b/_data/lit/lit_summary-penalty-over-years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gina Laptippytop\Documents\_git_repos\ghproj_ccgap\_data\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616C0CEE-F51A-41E9-96C0-2E744500A666}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C8C64-2756-4ABB-B203-E691965F2824}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F284945C-B536-4792-BD89-54D1A7087DE1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>years_in_corn</t>
   </si>
@@ -108,16 +108,116 @@
   </si>
   <si>
     <t>2-sites Minn</t>
+  </si>
+  <si>
+    <t>temps</t>
+  </si>
+  <si>
+    <t>precip</t>
+  </si>
+  <si>
+    <t>soil</t>
+  </si>
+  <si>
+    <t>Gentry et al. (2013)</t>
+  </si>
+  <si>
+    <t>unfertilized CC yield</t>
+  </si>
+  <si>
+    <t>AONR CC</t>
+  </si>
+  <si>
+    <t>AONR SC</t>
+  </si>
+  <si>
+    <t>crop CC</t>
+  </si>
+  <si>
+    <t>crop SC</t>
+  </si>
+  <si>
+    <t>crop general</t>
+  </si>
+  <si>
+    <t>yield at AONR CC</t>
+  </si>
+  <si>
+    <t>yield at AONR SC</t>
+  </si>
+  <si>
+    <t>Nresp CC</t>
+  </si>
+  <si>
+    <t>Nresp SC</t>
+  </si>
+  <si>
+    <t>CCgap at 0N</t>
+  </si>
+  <si>
+    <t>yield at 0N SC</t>
+  </si>
+  <si>
+    <t>GDD planting - 15 sept</t>
+  </si>
+  <si>
+    <t>Seifert et al. 2017</t>
+  </si>
+  <si>
+    <t>selected using MARS</t>
+  </si>
+  <si>
+    <t>drier districts have higher penalty</t>
+  </si>
+  <si>
+    <t>late planted corn = higher penalties</t>
+  </si>
+  <si>
+    <t>Corn prod index, slight relationship that as CSR goes up, penalty goes down</t>
+  </si>
+  <si>
+    <t>years in CC, more years = higher penalty</t>
+  </si>
+  <si>
+    <t>yield at 0N CC, higher value means lower penalty</t>
+  </si>
+  <si>
+    <t>(Nresp SC) - (Nresp CC), higher val = higher penalty</t>
+  </si>
+  <si>
+    <t>max T</t>
+  </si>
+  <si>
+    <t>VPD</t>
+  </si>
+  <si>
+    <t>min T, 61-90 DAP strongest</t>
+  </si>
+  <si>
+    <t>tillage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -139,12 +239,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,19 +885,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3571DFEC-2EAC-47F6-AAE2-490ED5BF3FEC}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="4" max="5" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,13 +911,16 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -738,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -749,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -760,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -771,7 +967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -782,7 +978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -795,11 +991,11 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -809,11 +1005,11 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -823,11 +1019,11 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -837,11 +1033,11 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -855,7 +1051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -866,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -877,7 +1073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -888,7 +1084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -899,7 +1095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1149,12 +1345,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251F1AAD-C394-4474-BC5D-07E9E9D498AB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>